<commit_message>
open xlsx format for compatibility
</commit_message>
<xml_diff>
--- a/src/main/java/com/aneonoir/dsalgo/practise/practisebook.xlsx
+++ b/src/main/java/com/aneonoir/dsalgo/practise/practisebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr dateCompatibility="0" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ab670958/IdeaProjects/my-coding-practise/src/main/java/com/aneonoir/dsalgo/practise/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E9B328B-05E0-4F4F-A979-5624012734DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{754B7563-AD9C-DD44-B287-7D45E21BA568}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16920" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,6 +37,9 @@
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -50,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="338">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="477" uniqueCount="338">
   <si>
     <t>Link</t>
   </si>
@@ -1079,7 +1082,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1159,19 +1162,19 @@
   </fills>
   <borders count="4">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <start style="thin">
         <color indexed="64"/>
-      </left>
-      <right style="thin">
+      </start>
+      <end style="thin">
         <color indexed="64"/>
-      </right>
+      </end>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1181,10 +1184,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <start/>
+      <end style="thin">
         <color indexed="64"/>
-      </right>
+      </end>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1194,10 +1197,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <start/>
+      <end style="thin">
         <color indexed="64"/>
-      </right>
+      </end>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1313,7 +1316,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1432,22 +1435,22 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:tint val="50%"/>
+                <a:satMod val="300%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="35%">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:tint val="37%"/>
+                <a:satMod val="300%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="15%"/>
+                <a:satMod val="350%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1455,18 +1458,18 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="130000"/>
+                <a:tint val="100%"/>
+                <a:shade val="100%"/>
+                <a:satMod val="130%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="50%"/>
+                <a:shade val="100%"/>
+                <a:satMod val="350%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1477,8 +1480,8 @@
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
+              <a:shade val="95%"/>
+              <a:satMod val="105%"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
@@ -1501,7 +1504,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="38%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1510,7 +1513,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
+                <a:alpha val="35%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1519,7 +1522,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
+                <a:alpha val="35%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1542,47 +1545,47 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="40%"/>
+                <a:satMod val="350%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="40%">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="45%"/>
+                <a:shade val="99%"/>
+                <a:satMod val="350%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="20%"/>
+                <a:satMod val="255%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect l="50%" t="-80%" r="50%" b="180%"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
+                <a:tint val="80%"/>
+                <a:satMod val="300%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
+                <a:shade val="30%"/>
+                <a:satMod val="200%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect l="50%" t="50%" r="50%" b="50%"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1633,7 +1636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D300"/>
   <sheetViews>
@@ -1802,7 +1805,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -2081,7 +2084,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -2112,7 +2115,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D200"/>
   <sheetViews>
@@ -2154,7 +2157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:D300"/>
   <sheetViews>
@@ -2196,7 +2199,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:D100"/>
   <sheetViews>
@@ -2239,7 +2242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:D300"/>
   <sheetViews>
@@ -2298,7 +2301,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -2335,7 +2338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -2369,7 +2372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:D500"/>
   <sheetViews>
@@ -2440,7 +2443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2469,7 +2472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D200"/>
   <sheetViews>
@@ -2541,7 +2544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2554,7 +2557,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2640,7 +2643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D200"/>
   <sheetViews>
@@ -2680,7 +2683,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D300"/>
   <sheetViews>
@@ -2728,7 +2731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E200"/>
   <sheetViews>
@@ -2791,7 +2794,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E537"/>
   <sheetViews>
@@ -3164,7 +3167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr transitionEvaluation="1" codeName="Sheet7"/>
   <dimension ref="A1:H159"/>
   <sheetViews>
@@ -3225,9 +3228,9 @@
       <c r="C7" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="13" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -3237,9 +3240,9 @@
       <c r="C8" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="13" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3249,9 +3252,9 @@
       <c r="C9" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="13" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -3261,9 +3264,9 @@
       <c r="C10" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="13" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3281,9 +3284,9 @@
       <c r="C12" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="13" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3296,9 +3299,9 @@
       <c r="C13" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="12" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -3320,9 +3323,9 @@
       <c r="C15" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="13" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -3348,9 +3351,9 @@
       <c r="C18" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="13" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
       <c r="H18" t="s">
         <v>320</v>
@@ -3363,9 +3366,9 @@
       <c r="C19" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="13" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -3384,9 +3387,9 @@
       <c r="C21" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="13" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -3396,9 +3399,9 @@
       <c r="C22" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="13" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -3418,9 +3421,9 @@
       <c r="C26" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="13" t="d">
         <f ca="1">NOW()</f>
-        <v>44022.5281181713</v>
+        <v>2020-07-10T12:47:58.64999973680824125</v>
       </c>
       <c r="H26" t="s">
         <v>334</v>
@@ -3457,7 +3460,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E401"/>
   <sheetViews>
@@ -4088,7 +4091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:D100"/>
   <sheetViews>

</xml_diff>

<commit_message>
added leetcode dynamic programing to the practisebook.xlsx and an easy dynamic programming.
</commit_message>
<xml_diff>
--- a/src/main/java/com/aneonoir/dsalgo/practise/practisebook.xlsx
+++ b/src/main/java/com/aneonoir/dsalgo/practise/practisebook.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="369">
   <si>
     <t xml:space="preserve">Questions</t>
   </si>
@@ -150,29 +150,19 @@
     <t xml:space="preserve">medium</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF99A8BA"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="13"/>
-        <color rgb="FF518843"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">https://leetcode.com/problems/range-sum-query-2d-immutable/</t>
-    </r>
+    <t xml:space="preserve"> https://leetcode.com/problems/range-sum-query-2d-immutable/</t>
   </si>
   <si>
     <t xml:space="preserve">Null handling, dynamic programming, there seems to be even faster way of calculating, than the used for loop. Check it out. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Range Sum Query - Immutable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/range-sum-query-immutable/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There seem to be having a better way , try learn it.</t>
   </si>
   <si>
     <t xml:space="preserve">Find the log base 2  value of a number</t>
@@ -1173,14 +1163,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="168" formatCode="dd/mm/yy\ hh:mm"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="169" formatCode="dd/mm/yy\ hh:mm"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1223,20 +1214,14 @@
       <color rgb="FF99A8BA"/>
       <name val="JetBrains Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
       <color rgb="FF99A8BA"/>
-      <name val=""/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="13"/>
-      <color rgb="FF518843"/>
-      <name val="JetBrains Mono"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="16"/>
@@ -1353,7 +1338,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1398,27 +1383,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1426,7 +1415,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1434,19 +1423,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1477,7 +1466,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF629755"/>
+      <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -1511,7 +1500,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF99A8BA"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF518843"/>
+      <rgbColor rgb="FF629755"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -1534,7 +1523,7 @@
       <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.83"/>
@@ -1728,269 +1717,269 @@
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="115.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -2015,19 +2004,19 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2053,7 +2042,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="123.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.83"/>
@@ -2062,17 +2051,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>345</v>
+      <c r="D1" s="14" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2102,7 +2091,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.17"/>
@@ -2111,22 +2100,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2151,31 +2140,31 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="66.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2200,30 +2189,30 @@
       <selection pane="topLeft" activeCell="A300" activeCellId="0" sqref="A300"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="95.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -2231,17 +2220,17 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -2266,25 +2255,25 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="69.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2310,22 +2299,22 @@
       <selection pane="topLeft" activeCell="N31" activeCellId="0" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2351,55 +2340,55 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>345</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>350</v>
+      <c r="A2" s="23" t="s">
+        <v>353</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>354</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>351</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B500" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2428,19 +2417,19 @@
       <selection pane="topLeft" activeCell="Q40" activeCellId="0" sqref="Q40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -2465,10 +2454,10 @@
       <selection pane="topLeft" activeCell="A200" activeCellId="0" sqref="A200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.16"/>
   </cols>
@@ -2543,7 +2532,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2566,7 +2555,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.17"/>
@@ -2575,62 +2564,62 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>358</v>
+      <c r="A2" s="23" t="s">
+        <v>361</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
-        <v>360</v>
+      <c r="A3" s="23" t="s">
+        <v>363</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
-        <v>361</v>
+      <c r="A4" s="23" t="s">
+        <v>364</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
-        <v>362</v>
+      <c r="A5" s="23" t="s">
+        <v>365</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
-        <v>364</v>
+      <c r="A6" s="24" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -2655,15 +2644,15 @@
   </sheetPr>
   <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="73.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="18.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="101.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="101.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2700,6 +2689,23 @@
         <v>44025</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="12" t="n">
+        <v>44025</v>
+      </c>
+    </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
         <v>26</v>
@@ -2707,7 +2713,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C14" r:id="rId1" display="https://leetcode.com/problems/range-sum-query-2d-immutable/"/>
+    <hyperlink ref="C14" r:id="rId1" display=" https://leetcode.com/problems/range-sum-query-2d-immutable/"/>
+    <hyperlink ref="C15" r:id="rId2" display="https://leetcode.com/problems/range-sum-query-immutable/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2730,31 +2737,31 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2784,49 +2791,49 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="85.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2854,259 +2861,259 @@
       <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="63.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="52.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>45</v>
+      <c r="E1" s="16" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3114,56 +3121,56 @@
     </row>
     <row r="37" customFormat="false" ht="187" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>85</v>
+        <v>87</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>89</v>
+        <v>49</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="13" t="s">
-        <v>95</v>
+      <c r="C43" s="15" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3234,344 +3241,344 @@
       <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="85.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>96</v>
+      <c r="E1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="18" t="n">
+        <v>103</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="19" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.904872295</v>
+        <v>44025.9122773075</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="E8" s="18" t="n">
+        <v>104</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="19" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9048723003</v>
+        <v>44025.9122773078</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="E9" s="18" t="n">
+      <c r="E9" s="19" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9048723005</v>
+        <v>44025.9122773079</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="18" t="n">
+        <v>106</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="19" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9048723006</v>
+        <v>44025.912277308</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="18" t="n">
+        <v>110</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="19" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9048723007</v>
+        <v>44025.9122773082</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="19" t="n">
+      <c r="C13" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="20" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9048723008</v>
+        <v>44025.9122773082</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" s="19"/>
+        <v>115</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="20"/>
     </row>
     <row r="15" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="18" t="n">
+        <v>116</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="19" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9048723009</v>
+        <v>44025.9122773084</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>114</v>
+        <v>118</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>114</v>
+        <v>119</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" s="18" t="n">
+        <v>120</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="19" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.904872301</v>
+        <v>44025.9122773085</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="E19" s="18" t="n">
+        <v>123</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" s="19" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9048723011</v>
+        <v>44025.9122773086</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="18"/>
+        <v>124</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E21" s="18" t="n">
+        <v>126</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" s="19" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9048723012</v>
+        <v>44025.9122773087</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E22" s="18" t="n">
+        <v>127</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" s="19" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9048723013</v>
+        <v>44025.9122773088</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="E26" s="20" t="n">
+        <v>130</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" s="21" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9048723014</v>
+        <v>44025.9122773089</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="E36" s="19" t="n">
+        <v>133</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" s="20" t="n">
         <v>44022</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E37" s="19" t="n">
+        <v>135</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" s="20" t="n">
         <v>44022</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>137</v>
+        <v>139</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>139</v>
+        <v>141</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>141</v>
+        <v>143</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>143</v>
+        <v>145</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>145</v>
+        <v>147</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>147</v>
+        <v>149</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>149</v>
+        <v>151</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3640,7 +3647,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="108"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.17"/>
@@ -3650,600 +3657,600 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C83" s="21" t="s">
-        <v>281</v>
+        <v>43</v>
+      </c>
+      <c r="C83" s="22" t="s">
+        <v>284</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -4277,31 +4284,31 @@
       <selection pane="topLeft" activeCell="A100" activeCellId="0" sqref="A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPdated few questions from leetcode,
</commit_message>
<xml_diff>
--- a/src/main/java/com/aneonoir/dsalgo/practise/practisebook.xlsx
+++ b/src/main/java/com/aneonoir/dsalgo/practise/practisebook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sorting" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,8 +39,33 @@
 </workbook>
 </file>
 
+<file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="E17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">A Bit of struggle, Try again to see if you can come
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="375">
   <si>
     <t xml:space="preserve">Questions</t>
   </si>
@@ -118,6 +143,13 @@
   </si>
   <si>
     <t xml:space="preserve">Follow up do better, Don't use any sorting algo. Rather try do it in place </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CanMakeArithmeticProgressionFromSequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* link: https://leetcode.com/problems/can-make-arithmetic-progression-from-sequence/
+</t>
   </si>
   <si>
     <t xml:space="preserve">Do reach here </t>
@@ -349,6 +381,12 @@
     <t xml:space="preserve">https://www.codewars.com/kata/5e2733f0e7432a000fb5ecc4/train/java</t>
   </si>
   <si>
+    <t xml:space="preserve">Generate Parentheses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/generate-parentheses/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Date</t>
   </si>
   <si>
@@ -1127,6 +1165,12 @@
   </si>
   <si>
     <t xml:space="preserve">codewars.com/kata/5679aa472b8f57fb8c000047/solutions/java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LuckyNumberInMatrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/lucky-numbers-in-a-matrix/</t>
   </si>
   <si>
     <t xml:space="preserve">Design Bloom Filter</t>
@@ -1171,7 +1215,7 @@
     <numFmt numFmtId="168" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="169" formatCode="dd/mm/yy\ hh:mm"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1217,6 +1261,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="13"/>
+      <color rgb="FF518843"/>
+      <name val="JetBrains Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="13"/>
       <color rgb="FF99A8BA"/>
       <name val="Calibri"/>
@@ -1235,6 +1287,20 @@
       <sz val="9"/>
       <color rgb="FF629755"/>
       <name val="Menlo"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF99A8BA"/>
+      <name val="JetBrains Mono"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1338,7 +1404,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1363,14 +1429,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1383,31 +1441,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1423,19 +1501,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1466,7 +1544,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF629755"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -1500,7 +1578,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF99A8BA"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF629755"/>
+      <rgbColor rgb="FF518843"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -1519,15 +1597,15 @@
   </sheetPr>
   <dimension ref="A1:F300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B33" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D28" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="110.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.67"/>
   </cols>
@@ -1685,9 +1763,23 @@
         <v>25</v>
       </c>
     </row>
+    <row r="40" customFormat="false" ht="29.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="8" t="n">
+        <v>44026</v>
+      </c>
+    </row>
     <row r="300" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1717,7 +1809,7 @@
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="115.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.67"/>
@@ -1725,13 +1817,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -1739,247 +1831,247 @@
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -2004,17 +2096,17 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -2042,7 +2134,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="123.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.83"/>
@@ -2052,21 +2144,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2091,7 +2183,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.17"/>
@@ -2101,13 +2193,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -2115,7 +2207,7 @@
     </row>
     <row r="300" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2140,7 +2232,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="66.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.83"/>
@@ -2150,13 +2242,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -2164,7 +2256,7 @@
     </row>
     <row r="100" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -2189,7 +2281,7 @@
       <selection pane="topLeft" activeCell="A300" activeCellId="0" sqref="A300"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="95.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.17"/>
@@ -2198,13 +2290,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -2212,7 +2304,7 @@
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -2220,17 +2312,17 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -2255,7 +2347,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="69.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.16"/>
@@ -2265,13 +2357,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -2299,20 +2391,20 @@
       <selection pane="topLeft" activeCell="N31" activeCellId="0" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -2334,67 +2426,82 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D500"/>
+  <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="72.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>353</v>
+      <c r="A2" s="26" t="s">
+        <v>357</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>357</v>
+      <c r="A3" s="26" t="s">
+        <v>361</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>358</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="E17" s="19" t="n">
+        <v>44027</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B500" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://leetcode.com/problems/find-all-numbers-disappeared-in-an-array/submissions/"/>
-    <hyperlink ref="D2" r:id="rId2" display="array/FindAllNumbersDisapearedInAnArray.java"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://leetcode.com/problems/find-all-numbers-disappeared-in-an-array/submissions/"/>
+    <hyperlink ref="D2" r:id="rId3" display="array/FindAllNumbersDisapearedInAnArray.java"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2403,6 +2510,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2417,19 +2525,19 @@
       <selection pane="topLeft" activeCell="Q40" activeCellId="0" sqref="Q40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -2454,7 +2562,7 @@
       <selection pane="topLeft" activeCell="A200" activeCellId="0" sqref="A200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.52"/>
@@ -2464,13 +2572,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -2478,7 +2586,7 @@
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -2486,7 +2594,7 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>5</v>
@@ -2494,7 +2602,7 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2502,12 +2610,12 @@
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2532,7 +2640,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2555,7 +2663,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.17"/>
@@ -2565,61 +2673,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>361</v>
+      <c r="A2" s="26" t="s">
+        <v>367</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>363</v>
+      <c r="A3" s="26" t="s">
+        <v>369</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
-        <v>364</v>
+      <c r="A4" s="26" t="s">
+        <v>370</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
-        <v>365</v>
+      <c r="A5" s="26" t="s">
+        <v>371</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
-        <v>367</v>
+      <c r="A6" s="27" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -2644,71 +2752,71 @@
   </sheetPr>
   <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="73.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="101.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>28</v>
+      <c r="C1" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>34</v>
+      <c r="A14" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="10" t="n">
+        <v>39</v>
+      </c>
+      <c r="F14" s="8" t="n">
         <v>44025</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>38</v>
+      <c r="A15" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>39</v>
+      <c r="C15" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="12" t="n">
+        <v>42</v>
+      </c>
+      <c r="F15" s="8" t="n">
         <v>44025</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2737,7 +2845,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.85"/>
@@ -2747,13 +2855,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -2761,12 +2869,12 @@
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2791,24 +2899,24 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="85.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -2816,24 +2924,24 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2855,13 +2963,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E537"/>
+  <dimension ref="A1:F537"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="63.33"/>
@@ -2871,249 +2979,249 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3121,61 +3229,75 @@
     </row>
     <row r="37" customFormat="false" ht="187" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F48" s="19" t="n">
+        <v>44027</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3241,11 +3363,11 @@
       <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="85.33"/>
@@ -3253,337 +3375,337 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>28</v>
+      <c r="C1" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>102</v>
+        <v>105</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="19" t="n">
+        <v>107</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9122773075</v>
+        <v>44027.2608468763</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E8" s="19" t="n">
+        <v>108</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9122773078</v>
+        <v>44027.2608468767</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E9" s="19" t="n">
+        <v>109</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9122773079</v>
+        <v>44027.2608468768</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" s="19" t="n">
+        <v>110</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.912277308</v>
+        <v>44027.2608468769</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="19" t="n">
+        <v>114</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9122773082</v>
+        <v>44027.260846877</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="20" t="n">
+      <c r="C13" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" s="23" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9122773082</v>
+        <v>44027.2608468771</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" s="20"/>
+        <v>119</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="E15" s="19" t="n">
+        <v>120</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9122773084</v>
+        <v>44027.2608468772</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>117</v>
+        <v>122</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>117</v>
+        <v>123</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" s="19" t="n">
+        <v>124</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9122773085</v>
+        <v>44027.2608468773</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="E19" s="19" t="n">
+        <v>127</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9122773086</v>
+        <v>44027.2608468774</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="E20" s="19"/>
+        <v>128</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="E21" s="19" t="n">
+        <v>130</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9122773087</v>
+        <v>44027.2608468775</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="E22" s="19" t="n">
+        <v>131</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9122773088</v>
+        <v>44027.2608468776</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="E26" s="21" t="n">
+        <v>134</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="24" t="n">
         <f aca="true">NOW()</f>
-        <v>44025.9122773089</v>
+        <v>44027.2608468777</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="E36" s="20" t="n">
+        <v>137</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" s="23" t="n">
         <v>44022</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="E37" s="20" t="n">
+        <v>139</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="23" t="n">
         <v>44022</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>138</v>
+        <v>141</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>140</v>
+        <v>143</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>144</v>
+        <v>147</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>146</v>
+        <v>149</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>148</v>
+        <v>151</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>150</v>
+        <v>153</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>152</v>
+        <v>155</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3647,7 +3769,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="108"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.17"/>
@@ -3658,13 +3780,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -3672,585 +3794,585 @@
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C83" s="22" t="s">
-        <v>284</v>
+        <v>45</v>
+      </c>
+      <c r="C83" s="25" t="s">
+        <v>288</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -4284,7 +4406,7 @@
       <selection pane="topLeft" activeCell="A100" activeCellId="0" sqref="A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.82"/>
@@ -4294,13 +4416,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -4308,7 +4430,7 @@
     </row>
     <row r="100" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
medium dynamic programming question added
</commit_message>
<xml_diff>
--- a/src/main/java/com/aneonoir/dsalgo/practise/practisebook.xlsx
+++ b/src/main/java/com/aneonoir/dsalgo/practise/practisebook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sorting" sheetId="1" state="visible" r:id="rId2"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="378">
   <si>
     <t xml:space="preserve">Questions</t>
   </si>
@@ -195,6 +195,15 @@
   </si>
   <si>
     <t xml:space="preserve">There seem to be having a better way , try learn it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IntegerBreak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/integer-break/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take care of the base cases, like for 2, 3 if they are precalculated, Don’t rush prove it </t>
   </si>
   <si>
     <t xml:space="preserve">Find the log base 2  value of a number</t>
@@ -1276,6 +1285,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="16"/>
       <color rgb="FFE26B0A"/>
       <name val="Calibri"/>
@@ -1295,14 +1312,6 @@
       <color rgb="FF99A8BA"/>
       <name val="JetBrains Mono"/>
       <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1457,19 +1466,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1477,15 +1486,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1505,7 +1514,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1816,262 +1825,262 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -2099,16 +2108,16 @@
   <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2143,17 +2152,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>352</v>
+      <c r="D1" s="16" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,22 +2201,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2241,22 +2250,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2289,22 +2298,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -2312,17 +2321,17 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -2356,16 +2365,16 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2397,16 +2406,16 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2441,61 +2450,61 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>358</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
-        <v>363</v>
+      <c r="A17" s="19" t="s">
+        <v>366</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>358</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>364</v>
-      </c>
-      <c r="E17" s="19" t="n">
+        <v>361</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="E17" s="14" t="n">
         <v>44027</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B500" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2532,12 +2541,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -2672,33 +2681,33 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>23</v>
@@ -2706,7 +2715,7 @@
     </row>
     <row r="4" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>23</v>
@@ -2714,20 +2723,20 @@
     </row>
     <row r="5" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="27" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -2752,8 +2761,8 @@
   </sheetPr>
   <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2812,6 +2821,23 @@
       </c>
       <c r="F15" s="8" t="n">
         <v>44025</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="14" t="n">
+        <v>44027</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2854,22 +2880,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2909,39 +2935,39 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2965,7 +2991,7 @@
   </sheetPr>
   <dimension ref="A1:F537"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
     </sheetView>
   </sheetViews>
@@ -2978,250 +3004,250 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>50</v>
+      <c r="E1" s="18" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3229,69 +3255,69 @@
     </row>
     <row r="37" customFormat="false" ht="187" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>94</v>
+        <v>54</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="15" t="s">
-        <v>100</v>
+      <c r="C43" s="17" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="17" t="s">
-        <v>101</v>
+      <c r="A48" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="F48" s="19" t="n">
+        <v>48</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F48" s="14" t="n">
         <v>44027</v>
       </c>
     </row>
@@ -3374,255 +3400,255 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>103</v>
+      <c r="E1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E7" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.2608468763</v>
+        <v>44027.3546729752</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E8" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.2608468767</v>
+        <v>44027.3546729755</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>106</v>
       </c>
       <c r="E9" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.2608468768</v>
+        <v>44027.3546729756</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E10" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.2608468769</v>
+        <v>44027.3546729757</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E12" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.260846877</v>
+        <v>44027.3546729758</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>113</v>
-      </c>
       <c r="C13" s="21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E13" s="23" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.2608468771</v>
+        <v>44027.3546729759</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E15" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.2608468772</v>
+        <v>44027.3546729761</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E18" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.2608468773</v>
+        <v>44027.3546729762</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E19" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.2608468774</v>
+        <v>44027.3546729763</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E21" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.2608468775</v>
+        <v>44027.3546729764</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E22" s="22" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.2608468776</v>
+        <v>44027.3546729765</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E26" s="24" t="n">
         <f aca="true">NOW()</f>
-        <v>44027.2608468777</v>
+        <v>44027.3546729766</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E36" s="23" t="n">
         <v>44022</v>
@@ -3630,10 +3656,10 @@
     </row>
     <row r="37" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E37" s="23" t="n">
         <v>44022</v>
@@ -3641,66 +3667,66 @@
     </row>
     <row r="38" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3779,600 +3805,600 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C83" s="25" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -4415,22 +4441,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>